<commit_message>
make 2d topo strings only
</commit_message>
<xml_diff>
--- a/GPS_ERT.xlsx
+++ b/GPS_ERT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fnk\PycharmProjects\Resipy_interpolate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B12A3EE6-EB1F-49AD-8400-A29728D911A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF98F361-B2F3-4A63-8B52-90CE2D3B5C5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{D282C34C-2F99-4660-AFC3-F49C62DCE88E}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D282C34C-2F99-4660-AFC3-F49C62DCE88E}"/>
   </bookViews>
   <sheets>
     <sheet name="ERT_A_1m" sheetId="3" r:id="rId1"/>
@@ -419,8 +419,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43A6722C-2401-4FFC-B0F6-091BF03F7B5A}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -446,10 +446,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="3">
-        <v>613183.30000000005</v>
+        <v>613087</v>
       </c>
       <c r="C2" s="3">
-        <v>6651210.7999999998</v>
+        <v>6651252</v>
       </c>
       <c r="D2" s="3">
         <v>130.90799999999999</v>
@@ -939,15 +939,15 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCEEAC10-5ACE-4994-8C51-F14EF567726F}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -961,7 +961,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -975,7 +975,7 @@
         <v>150.822</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>11</v>
       </c>
@@ -988,8 +988,16 @@
       <c r="D3">
         <v>147.809</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <f t="shared" ref="E3:E7" si="0">SQRT((B3-B2)^2+(C3-C2)^2)</f>
+        <v>53.498130808280862</v>
+      </c>
+      <c r="F3">
+        <f>E3/(A3-A2)</f>
+        <v>5.3498130808280866</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>48</v>
       </c>
@@ -1002,8 +1010,16 @@
       <c r="D4">
         <v>129.04499999999999</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>186.11007495565707</v>
+      </c>
+      <c r="F4">
+        <f t="shared" ref="F4:F8" si="1">E4/(A4-A3)</f>
+        <v>5.0300020258285691</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>57</v>
       </c>
@@ -1016,8 +1032,16 @@
       <c r="D5">
         <v>126.922</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>46.02781767583518</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>5.1142019639816869</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>74</v>
       </c>
@@ -1030,8 +1054,16 @@
       <c r="D6">
         <v>124.833</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>83.653810432865001</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>4.9208123784038236</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>76</v>
       </c>
@@ -1044,8 +1076,16 @@
       <c r="D7">
         <v>124.624</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>10.017983829093161</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>5.0089919145465807</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>80</v>
       </c>
@@ -1057,6 +1097,14 @@
       </c>
       <c r="D8">
         <v>124.565</v>
+      </c>
+      <c r="E8">
+        <f>SQRT((B8-B7)^2+(C8-C7)^2)</f>
+        <v>18.317477993085113</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>4.5793694982712783</v>
       </c>
     </row>
   </sheetData>
@@ -1292,10 +1340,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE16C4F5-4F30-4065-8EAF-D305BA9AB2DB}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1333,127 +1381,57 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="B3">
-        <v>613049.80000000005</v>
+        <v>613184.5</v>
       </c>
       <c r="C3">
-        <v>6651240.5999999996</v>
+        <v>6651268.4000000004</v>
       </c>
       <c r="D3">
-        <v>130.678</v>
+        <v>134.48099999999999</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>13</v>
-      </c>
-      <c r="B4">
-        <v>612950.30000000005</v>
+        <v>32</v>
+      </c>
+      <c r="B4" s="1">
+        <v>613198</v>
       </c>
       <c r="C4">
-        <v>6651307.2000000002</v>
+        <v>6651272.2000000002</v>
       </c>
       <c r="D4">
-        <v>131.27500000000001</v>
+        <v>133.316</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="B5">
-        <v>613140.69999999995</v>
-      </c>
-      <c r="C5" s="1">
-        <v>6651259</v>
+        <v>613221.6</v>
+      </c>
+      <c r="C5">
+        <v>6651278.7999999998</v>
       </c>
       <c r="D5">
-        <v>131.96100000000001</v>
+        <v>133.53200000000001</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="B6">
-        <v>613121.30000000005</v>
+        <v>613277.4</v>
       </c>
       <c r="C6">
-        <v>6651226.4000000004</v>
+        <v>6651289.5</v>
       </c>
       <c r="D6">
-        <v>132.30799999999999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>26</v>
-      </c>
-      <c r="B7">
-        <v>613168.80000000005</v>
-      </c>
-      <c r="C7">
-        <v>6651263.5</v>
-      </c>
-      <c r="D7">
-        <v>133.286</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>28</v>
-      </c>
-      <c r="B8">
-        <v>613184.5</v>
-      </c>
-      <c r="C8">
-        <v>6651268.4000000004</v>
-      </c>
-      <c r="D8">
-        <v>134.48099999999999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>32</v>
-      </c>
-      <c r="B9" s="1">
-        <v>613198</v>
-      </c>
-      <c r="C9">
-        <v>6651272.2000000002</v>
-      </c>
-      <c r="D9">
-        <v>133.316</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>37</v>
-      </c>
-      <c r="B10">
-        <v>613221.6</v>
-      </c>
-      <c r="C10">
-        <v>6651278.7999999998</v>
-      </c>
-      <c r="D10">
-        <v>133.53200000000001</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>48</v>
-      </c>
-      <c r="B11">
-        <v>613277.4</v>
-      </c>
-      <c r="C11">
-        <v>6651289.5</v>
-      </c>
-      <c r="D11">
         <v>135.209</v>
       </c>
     </row>
@@ -1622,7 +1600,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1660,7 +1638,7 @@
         <v>96</v>
       </c>
       <c r="B3">
-        <v>6113148.5999999996</v>
+        <v>613148.6</v>
       </c>
       <c r="C3">
         <v>6651182.2000000002</v>
@@ -1678,8 +1656,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDCB8BA7-C14C-4117-A5F3-3301CE23DEFC}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1748,7 +1726,7 @@
         <v>612979.69999999995</v>
       </c>
       <c r="C5">
-        <v>66511267</v>
+        <v>6651267</v>
       </c>
       <c r="D5">
         <v>126.753</v>
@@ -1818,7 +1796,7 @@
         <v>613135.9</v>
       </c>
       <c r="C10">
-        <v>665187.19999999995</v>
+        <v>6651187.2000000002</v>
       </c>
       <c r="D10">
         <v>134.38900000000001</v>

</xml_diff>